<commit_message>
datove_sady_nakres: add new table primary_final
</commit_message>
<xml_diff>
--- a/engeto_datove_sady_nakres.xlsx
+++ b/engeto_datove_sady_nakres.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucka\Documents\___dokumenty_nase\_lucka\IT\__analytika\engeto_projekt_SQL\projekt_SQL_engeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC3981A-090C-4828-9BB1-D495877918B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB62934-4976-467D-8C06-AB2472BEB035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AF0EFDAF-211C-4303-A2B0-919BFF3D9538}"/>
   </bookViews>
   <sheets>
-    <sheet name="czechia_payroll" sheetId="2" r:id="rId1"/>
+    <sheet name="primary_final" sheetId="3" r:id="rId1"/>
+    <sheet name="czechia_payroll" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="147">
   <si>
     <t>name</t>
   </si>
@@ -542,6 +543,72 @@
       <t xml:space="preserve"> = přepočtený - viz. níže</t>
     </r>
   </si>
+  <si>
+    <t>cp.ip_code</t>
+  </si>
+  <si>
+    <t>cpip_name</t>
+  </si>
+  <si>
+    <t>cp.payroll_year</t>
+  </si>
+  <si>
+    <t>payroll</t>
+  </si>
+  <si>
+    <t>247 položek (19*13)</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>cp.code</t>
+  </si>
+  <si>
+    <t>cpc.name</t>
+  </si>
+  <si>
+    <t>Rýže …</t>
+  </si>
+  <si>
+    <t>cp.avg_value</t>
+  </si>
+  <si>
+    <t>cp.avg_value_category</t>
+  </si>
+  <si>
+    <t>cp.date_from</t>
+  </si>
+  <si>
+    <t>name_category</t>
+  </si>
+  <si>
+    <t>price_year</t>
+  </si>
+  <si>
+    <t>ip_code</t>
+  </si>
+  <si>
+    <t>avg_payroll_year</t>
+  </si>
+  <si>
+    <t>ip_name</t>
+  </si>
+  <si>
+    <t>price = cpe</t>
+  </si>
+  <si>
+    <t>payroll = cpl</t>
+  </si>
+  <si>
+    <t>value_price</t>
+  </si>
+  <si>
+    <t>342 položek (27*13-9)</t>
+  </si>
+  <si>
+    <t>primary final</t>
+  </si>
 </sst>
 </file>
 
@@ -550,7 +617,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,8 +662,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -645,8 +720,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -938,11 +1019,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1044,6 +1140,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1364,11 +1471,246 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E898D9E-8E92-4F10-8946-2228D4042393}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="54">
+        <v>111101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="54">
+        <v>14817.75</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" s="54">
+        <v>21.29</v>
+      </c>
+      <c r="G4" s="58" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="59">
+        <v>2006</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="59">
+        <v>2006</v>
+      </c>
+      <c r="G5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="58" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="58" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11"/>
+      <c r="E11" s="3"/>
+      <c r="G11"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="30"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="54">
+        <v>14817.75</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="59">
+        <v>2006</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="57" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17" s="54">
+        <v>111101</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="54">
+        <v>21.29</v>
+      </c>
+      <c r="C19" s="58" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="2"/>
+      <c r="G24"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.47244094488188981" right="0.47244094488188981" top="0.47244094488188981" bottom="0.47244094488188981" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4156B1D-D0A4-4A49-A4DD-B0E459D73A01}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1419,7 +1761,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="13">
-        <v>741371809</v>
+        <v>741381972</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>17</v>
@@ -1451,7 +1793,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="14">
-        <v>154</v>
+        <v>9017</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>0</v>
@@ -1480,7 +1822,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="14">
-        <v>316</v>
+        <v>5958</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>121</v>
@@ -1507,7 +1849,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="14">
-        <v>80403</v>
+        <v>200</v>
       </c>
       <c r="G5" s="35" t="s">
         <v>44</v>
@@ -1530,7 +1872,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="14">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>31</v>
@@ -1588,7 +1930,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="48">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
datove_sady_nakres: new suggest for JOINing four tables
</commit_message>
<xml_diff>
--- a/engeto_datove_sady_nakres.xlsx
+++ b/engeto_datove_sady_nakres.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucka\Documents\___dokumenty_nase\_lucka\IT\__analytika\engeto_projekt_SQL\projekt_SQL_engeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB62934-4976-467D-8C06-AB2472BEB035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C57A12C-699E-4EA0-B923-9CD75EE580DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AF0EFDAF-211C-4303-A2B0-919BFF3D9538}"/>
   </bookViews>
   <sheets>
-    <sheet name="primary_final" sheetId="3" r:id="rId1"/>
-    <sheet name="czechia_payroll" sheetId="2" r:id="rId2"/>
+    <sheet name="nove_spojovani" sheetId="4" r:id="rId1"/>
+    <sheet name="primary_final" sheetId="3" r:id="rId2"/>
+    <sheet name="czechia_payroll" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="151">
   <si>
     <t>name</t>
   </si>
@@ -608,6 +609,18 @@
   </si>
   <si>
     <t>primary final</t>
+  </si>
+  <si>
+    <t>czechia_price = CPE</t>
+  </si>
+  <si>
+    <t>czechia_payroll = CPL</t>
+  </si>
+  <si>
+    <t>czechia_price_category = CPC</t>
+  </si>
+  <si>
+    <t>czechia_payroll_industry_branch = CPIB</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1051,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1147,7 +1160,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1471,10 +1483,210 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD0BFEC-6863-4AFF-B32A-C595975C5F54}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="13">
+        <v>741381972</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="22">
+        <v>770138309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="14">
+        <v>9017</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="26">
+        <v>142.62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="14">
+        <v>5958</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="26">
+        <v>112704</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="14">
+        <v>200</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="14">
+        <v>200</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="48">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D11"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="22">
+        <v>112704</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.47244094488188981" right="0.47244094488188981" top="0.47244094488188981" bottom="0.47244094488188981" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E898D9E-8E92-4F10-8946-2228D4042393}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
@@ -1520,7 +1732,7 @@
       <c r="C2" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="56" t="s">
         <v>131</v>
       </c>
       <c r="F2" s="54">
@@ -1537,7 +1749,7 @@
       <c r="B3" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" t="s">
         <v>141</v>
       </c>
       <c r="E3" s="55" t="s">
@@ -1557,7 +1769,7 @@
       <c r="B4" s="54">
         <v>14817.75</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" t="s">
         <v>140</v>
       </c>
       <c r="E4" s="55" t="s">
@@ -1566,7 +1778,7 @@
       <c r="F4" s="54">
         <v>21.29</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="57" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1574,16 +1786,16 @@
       <c r="A5" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="58">
         <v>2006</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="55" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="59">
+      <c r="F5" s="58">
         <v>2006</v>
       </c>
       <c r="G5" t="s">
@@ -1594,12 +1806,12 @@
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="57" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="57" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1634,7 +1846,7 @@
       <c r="B14" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1645,7 +1857,7 @@
       <c r="B15" s="54">
         <v>14817.75</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1653,15 +1865,15 @@
       <c r="A16" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="B16" s="59">
+      <c r="B16" s="58">
         <v>2006</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="56" t="s">
         <v>131</v>
       </c>
       <c r="B17" s="54">
@@ -1689,7 +1901,7 @@
       <c r="B19" s="54">
         <v>21.29</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="57" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1705,7 +1917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4156B1D-D0A4-4A49-A4DD-B0E459D73A01}">
   <dimension ref="A1:L34"/>
   <sheetViews>

</xml_diff>

<commit_message>
datove_sady_nakres: first change table primary_final
</commit_message>
<xml_diff>
--- a/engeto_datove_sady_nakres.xlsx
+++ b/engeto_datove_sady_nakres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucka\Documents\___dokumenty_nase\_lucka\IT\__analytika\engeto_projekt_SQL\projekt_SQL_engeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C57A12C-699E-4EA0-B923-9CD75EE580DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EA236C-0F52-4D6E-BCC1-42C8652C4744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AF0EFDAF-211C-4303-A2B0-919BFF3D9538}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="170">
   <si>
     <t>name</t>
   </si>
@@ -596,12 +596,6 @@
     <t>ip_name</t>
   </si>
   <si>
-    <t>price = cpe</t>
-  </si>
-  <si>
-    <t>payroll = cpl</t>
-  </si>
-  <si>
     <t>value_price</t>
   </si>
   <si>
@@ -611,16 +605,223 @@
     <t>primary final</t>
   </si>
   <si>
-    <t>czechia_price = CPE</t>
-  </si>
-  <si>
-    <t>czechia_payroll = CPL</t>
-  </si>
-  <si>
-    <t>czechia_price_category = CPC</t>
-  </si>
-  <si>
-    <t>czechia_payroll_industry_branch = CPIB</t>
+    <t>13let x 19branch</t>
+  </si>
+  <si>
+    <t>13let x 27category -9</t>
+  </si>
+  <si>
+    <t>cpe.date_from</t>
+  </si>
+  <si>
+    <t>(1)</t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(4)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2017</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-11-13 00:00:00.000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>cpl.value AS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>avg_payroll_year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>cpl.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>payroll_year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>cpe.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>category_code</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cpe.value AS </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>value_price</t>
+    </r>
+  </si>
+  <si>
+    <t>1. czechia_payroll = CPL</t>
+  </si>
+  <si>
+    <t>2. czechia_price = CPE</t>
+  </si>
+  <si>
+    <t>3. czechia_payroll_industry_branch = CPIB</t>
+  </si>
+  <si>
+    <t>4.czechia_price_category = CPC</t>
+  </si>
+  <si>
+    <t>cpib_name</t>
+  </si>
+  <si>
+    <t>cp.ib_code</t>
+  </si>
+  <si>
+    <t>ib_code</t>
+  </si>
+  <si>
+    <t>ib_name</t>
+  </si>
+  <si>
+    <r>
+      <t>cpl.industry_branch_code AS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ib_code</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cpib.name AS </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ib.name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>cpc.name AS</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> category_name</t>
+    </r>
+  </si>
+  <si>
+    <t>6498 řádků:</t>
+  </si>
+  <si>
+    <t>19 industries x 13 years x 26 categories = 6422</t>
+  </si>
+  <si>
+    <t>19 industries x 4 years x 1 category = 76</t>
   </si>
 </sst>
 </file>
@@ -630,7 +831,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,8 +884,43 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -739,8 +975,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1047,11 +1289,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1165,6 +1420,27 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -1484,196 +1760,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD0BFEC-6863-4AFF-B32A-C595975C5F54}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1"/>
+      <c r="H1" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="14">
+        <v>9017</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="26">
+        <v>142.62</v>
+      </c>
+      <c r="G2" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="62">
+        <v>112704</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="26">
+        <v>112704</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="48">
+        <v>2000</v>
+      </c>
+      <c r="D4" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>147</v>
+      </c>
+      <c r="F4" s="66" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D8" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="E8" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="B2" s="13">
-        <v>741381972</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="22">
-        <v>770138309</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="14">
-        <v>9017</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="26">
-        <v>142.62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="14">
-        <v>5958</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="26">
-        <v>112704</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="14">
-        <v>200</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="14">
-        <v>200</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="48">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D11"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="22">
-        <v>112704</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="15" t="s">
+      <c r="E9" s="59" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>21</v>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1687,7 +1939,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1716,7 +1968,7 @@
         <v>130</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G1"/>
       <c r="H1" s="3"/>
@@ -1744,7 +1996,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="55" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="B3" s="54" t="s">
         <v>80</v>
@@ -1778,8 +2030,8 @@
       <c r="F4" s="54">
         <v>21.29</v>
       </c>
-      <c r="G4" s="57" t="s">
-        <v>144</v>
+      <c r="G4" s="69" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1806,14 +2058,10 @@
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="57" t="s">
-        <v>142</v>
-      </c>
+      <c r="A7" s="57"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
-        <v>143</v>
-      </c>
+      <c r="A8" s="57"/>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11"/>
@@ -1824,19 +2072,19 @@
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B12" s="30"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="53" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="B13" s="54" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1847,7 +2095,7 @@
         <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1902,7 +2150,7 @@
         <v>21.29</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1922,7 +2170,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="D17" sqref="D17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
datove_sady_nakres: create design of new table primary_final
</commit_message>
<xml_diff>
--- a/engeto_datove_sady_nakres.xlsx
+++ b/engeto_datove_sady_nakres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucka\Documents\___dokumenty_nase\_lucka\IT\__analytika\engeto_projekt_SQL\projekt_SQL_engeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EA236C-0F52-4D6E-BCC1-42C8652C4744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2419D09-D1DE-44F8-8D13-7BAB2B12C5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AF0EFDAF-211C-4303-A2B0-919BFF3D9538}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="171">
   <si>
     <t>name</t>
   </si>
@@ -679,23 +679,6 @@
   </si>
   <si>
     <r>
-      <t>cpl.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>payroll_year</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>cpe.</t>
     </r>
     <r>
@@ -822,6 +805,48 @@
   </si>
   <si>
     <t>19 industries x 4 years x 1 category = 76</t>
+  </si>
+  <si>
+    <r>
+      <t>cpl.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>payroll_year</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AS year</t>
+    </r>
+  </si>
+  <si>
+    <t>TABLE primary_final</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1441,6 +1466,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -1760,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD0BFEC-6863-4AFF-B32A-C595975C5F54}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection sqref="A1:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1781,20 +1810,20 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>145</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>146</v>
       </c>
       <c r="G1"/>
       <c r="H1" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>22</v>
@@ -1814,7 +1843,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F2" s="26">
         <v>142.62</v>
@@ -1834,7 +1863,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="67" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>10</v>
@@ -1843,7 +1872,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F3" s="26">
         <v>112704</v>
@@ -1852,7 +1881,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I3" s="26" t="s">
         <v>20</v>
@@ -1863,7 +1892,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="C4" s="48">
         <v>2000</v>
@@ -1884,14 +1913,20 @@
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>166</v>
+      </c>
       <c r="E7" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="D8" s="63" t="s">
         <v>148</v>
       </c>
@@ -1903,29 +1938,99 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" s="59" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F9" s="60" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>167</v>
+      <c r="B11" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>168</v>
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="70" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="54">
+        <v>9017</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" s="55" t="s">
         <v>169</v>
+      </c>
+      <c r="C15" s="71">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" s="54">
+        <v>112704</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="54">
+        <v>142.62</v>
       </c>
     </row>
   </sheetData>
@@ -1996,7 +2101,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="55" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" s="54" t="s">
         <v>80</v>
@@ -2078,13 +2183,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B13" s="54" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2095,7 +2200,7 @@
         <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>